<commit_message>
to chage background image
</commit_message>
<xml_diff>
--- a/zipdb.xlsx
+++ b/zipdb.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="96" windowWidth="18312" windowHeight="11652" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="96" windowWidth="18312" windowHeight="11652" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="sido" sheetId="3" r:id="rId1"/>
     <sheet name="gungu" sheetId="1" r:id="rId2"/>
     <sheet name="dong" sheetId="2" r:id="rId3"/>
+    <sheet name="sejong" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12552" uniqueCount="5119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12576" uniqueCount="5120">
   <si>
     <t>서울</t>
   </si>
@@ -15378,6 +15379,10 @@
   </si>
   <si>
     <t>gugun</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>세종시</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -16433,8 +16438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B275"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76:B99"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77:B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -17046,121 +17051,193 @@
       <c r="A76" t="s">
         <v>2070</v>
       </c>
+      <c r="B76" t="s">
+        <v>5119</v>
+      </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>2070</v>
       </c>
+      <c r="B77" t="s">
+        <v>5119</v>
+      </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>2070</v>
       </c>
+      <c r="B78" t="s">
+        <v>5119</v>
+      </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>2070</v>
       </c>
+      <c r="B79" t="s">
+        <v>5119</v>
+      </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B80" t="s">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B81" t="s">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B82" t="s">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B83" t="s">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B84" t="s">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B85" t="s">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B86" t="s">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B87" t="s">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B88" t="s">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B89" t="s">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B90" t="s">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B91" t="s">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B92" t="s">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B93" t="s">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B94" t="s">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B95" t="s">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
         <v>2070</v>
+      </c>
+      <c r="B96" t="s">
+        <v>5119</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
         <v>2070</v>
       </c>
+      <c r="B97" t="s">
+        <v>5119</v>
+      </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>2070</v>
       </c>
+      <c r="B98" t="s">
+        <v>5119</v>
+      </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
         <v>2070</v>
       </c>
+      <c r="B99" t="s">
+        <v>5119</v>
+      </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
@@ -18573,15 +18650,16 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6004"/>
+  <dimension ref="A1:B5980"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5979" workbookViewId="0">
-      <selection activeCell="A6004" sqref="A5982:A6004"/>
+    <sheetView topLeftCell="A5974" workbookViewId="0">
+      <selection activeCell="A5981" sqref="A5981:B6004"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -66426,195 +66504,211 @@
         <v>5113</v>
       </c>
     </row>
-    <row r="5981" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5981" t="s">
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
         <v>5118</v>
       </c>
-      <c r="B5981" t="s">
+      <c r="B1" t="s">
         <v>2071</v>
       </c>
     </row>
-    <row r="5982" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5982" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>5118</v>
       </c>
-      <c r="B5982" t="s">
+      <c r="B2" t="s">
         <v>2072</v>
       </c>
     </row>
-    <row r="5983" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5983" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>5118</v>
       </c>
-      <c r="B5983" t="s">
+      <c r="B3" t="s">
         <v>2073</v>
       </c>
     </row>
-    <row r="5984" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5984" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
         <v>5118</v>
       </c>
-      <c r="B5984" t="s">
+      <c r="B4" t="s">
         <v>2074</v>
       </c>
     </row>
-    <row r="5985" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5985" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>5118</v>
       </c>
-      <c r="B5985" t="s">
+      <c r="B5" t="s">
         <v>2075</v>
       </c>
     </row>
-    <row r="5986" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5986" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>5118</v>
       </c>
-      <c r="B5986" t="s">
+      <c r="B6" t="s">
         <v>2076</v>
       </c>
     </row>
-    <row r="5987" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5987" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>5118</v>
       </c>
-      <c r="B5987" t="s">
+      <c r="B7" t="s">
         <v>2077</v>
       </c>
     </row>
-    <row r="5988" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5988" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>5118</v>
       </c>
-      <c r="B5988" t="s">
+      <c r="B8" t="s">
         <v>2078</v>
       </c>
     </row>
-    <row r="5989" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5989" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
         <v>5118</v>
       </c>
-      <c r="B5989" t="s">
+      <c r="B9" t="s">
         <v>2079</v>
       </c>
     </row>
-    <row r="5990" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5990" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>5118</v>
       </c>
-      <c r="B5990" t="s">
+      <c r="B10" t="s">
         <v>2080</v>
       </c>
     </row>
-    <row r="5991" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5991" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
         <v>5118</v>
       </c>
-      <c r="B5991" t="s">
+      <c r="B11" t="s">
         <v>2081</v>
       </c>
     </row>
-    <row r="5992" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5992" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
         <v>5118</v>
       </c>
-      <c r="B5992" t="s">
+      <c r="B12" t="s">
         <v>2082</v>
       </c>
     </row>
-    <row r="5993" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5993" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
         <v>5118</v>
       </c>
-      <c r="B5993" t="s">
+      <c r="B13" t="s">
         <v>2083</v>
       </c>
     </row>
-    <row r="5994" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5994" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
         <v>5118</v>
       </c>
-      <c r="B5994" t="s">
+      <c r="B14" t="s">
         <v>2084</v>
       </c>
     </row>
-    <row r="5995" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5995" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
         <v>5118</v>
       </c>
-      <c r="B5995" t="s">
+      <c r="B15" t="s">
         <v>2085</v>
       </c>
     </row>
-    <row r="5996" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5996" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
         <v>5118</v>
       </c>
-      <c r="B5996" t="s">
+      <c r="B16" t="s">
         <v>2086</v>
       </c>
     </row>
-    <row r="5997" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5997" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
         <v>5118</v>
       </c>
-      <c r="B5997" t="s">
+      <c r="B17" t="s">
         <v>2087</v>
       </c>
     </row>
-    <row r="5998" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5998" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
         <v>5118</v>
       </c>
-      <c r="B5998" t="s">
+      <c r="B18" t="s">
         <v>2088</v>
       </c>
     </row>
-    <row r="5999" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5999" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
         <v>5118</v>
       </c>
-      <c r="B5999" t="s">
+      <c r="B19" t="s">
         <v>2089</v>
       </c>
     </row>
-    <row r="6000" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6000" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>5118</v>
       </c>
-      <c r="B6000" t="s">
+      <c r="B20" t="s">
         <v>2090</v>
       </c>
     </row>
-    <row r="6001" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6001" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
         <v>5118</v>
       </c>
-      <c r="B6001" t="s">
+      <c r="B21" t="s">
         <v>2091</v>
       </c>
     </row>
-    <row r="6002" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6002" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
         <v>5118</v>
       </c>
-      <c r="B6002" t="s">
+      <c r="B22" t="s">
         <v>2092</v>
       </c>
     </row>
-    <row r="6003" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6003" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
         <v>5118</v>
       </c>
-      <c r="B6003" t="s">
+      <c r="B23" t="s">
         <v>2093</v>
       </c>
     </row>
-    <row r="6004" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6004" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
         <v>5118</v>
       </c>
-      <c r="B6004" t="s">
+      <c r="B24" t="s">
         <v>2094</v>
       </c>
     </row>

</xml_diff>